<commit_message>
Se actualiza  ejemplo con todo lo visto en la segunda unidad del curso
</commit_message>
<xml_diff>
--- a/src/test/resources/data/DataPruebas.xlsx
+++ b/src/test/resources/data/DataPruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\domingo.saavedra\Desktop\IntroSelenium\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{369193C5-FD2F-4509-976C-184A57464B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02A895C-8033-42B8-9F8E-029D85B5DF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -181,7 +181,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>userSecuritydfsdaf009@gmail.com</t>
+    <t>userSecuritefgsdydfsdaf009@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>